<commit_message>
Upload Y4_B2526_Quiz_Pediatrics_schedule.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/modules_schedules/Y4_B2526_Quiz_Pediatrics_schedule.xlsx
+++ b/modules_schedules/Y4_B2526_Quiz_Pediatrics_schedule.xlsx
@@ -463,7 +463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -535,12 +535,12 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>06/09/2025</t>
+          <t>07/09/2025</t>
         </is>
       </c>
       <c r="F2" s="4" t="inlineStr">
@@ -560,7 +560,7 @@
       </c>
       <c r="B3" s="6" t="inlineStr">
         <is>
-          <t>PED-B2-2</t>
+          <t>PED-B2-1</t>
         </is>
       </c>
       <c r="C3" s="6" t="inlineStr">
@@ -595,7 +595,7 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>PED-B2-3</t>
+          <t>PED-B2-2</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
@@ -630,7 +630,7 @@
       </c>
       <c r="B5" s="6" t="inlineStr">
         <is>
-          <t>PED-B2-4</t>
+          <t>PED-B2-3</t>
         </is>
       </c>
       <c r="C5" s="6" t="inlineStr">
@@ -665,7 +665,7 @@
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>PED-B2-5</t>
+          <t>PED-B2-4</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
@@ -700,30 +700,65 @@
       </c>
       <c r="B7" s="6" t="inlineStr">
         <is>
+          <t>PED-B2-5</t>
+        </is>
+      </c>
+      <c r="C7" s="6" t="inlineStr">
+        <is>
+          <t>pediatrics</t>
+        </is>
+      </c>
+      <c r="D7" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E7" s="7" t="inlineStr">
+        <is>
+          <t>06/09/2025</t>
+        </is>
+      </c>
+      <c r="F7" s="8" t="inlineStr">
+        <is>
+          <t>08:00:00</t>
+        </is>
+      </c>
+      <c r="G7" s="9" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
           <t>PED-B2-6</t>
         </is>
       </c>
-      <c r="C7" s="6" t="inlineStr">
+      <c r="C8" s="2" t="inlineStr">
         <is>
           <t>pediatrics</t>
         </is>
       </c>
-      <c r="D7" s="6" t="inlineStr">
+      <c r="D8" s="2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E7" s="7" t="inlineStr">
+      <c r="E8" s="3" t="inlineStr">
         <is>
           <t>06/09/2025</t>
         </is>
       </c>
-      <c r="F7" s="8" t="inlineStr">
+      <c r="F8" s="4" t="inlineStr">
         <is>
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G7" s="9" t="n">
+      <c r="G8" s="5" t="n">
         <v>120</v>
       </c>
     </row>

</xml_diff>